<commit_message>
Excel extraction is working, simple selection of the first sheet.
</commit_message>
<xml_diff>
--- a/src/test/resources/se/simonsoft/cms/indexing/keydef/Techdata1.xlsx
+++ b/src/test/resources/se/simonsoft/cms/indexing/keydef/Techdata1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takesson/git/cms-indexing-keydef/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/takesson/git/cms-indexing-keydef/src/test/resources/se/simonsoft/cms/indexing/keydef/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="28200" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="2040" yWindow="820" windowWidth="28200" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="First sheet" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Just</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Key</t>
+  </si>
+  <si>
+    <t>ProductionDate</t>
+  </si>
+  <si>
+    <t>ProductionDateText</t>
+  </si>
+  <si>
+    <t>2016-02-01</t>
   </si>
 </sst>
 </file>
@@ -153,17 +162,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,9 +453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -465,8 +479,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>6</v>
+      <c r="B2" s="6">
+        <v>6000</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -515,6 +529,22 @@
       </c>
       <c r="C6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4">
+        <v>42429</v>
       </c>
     </row>
   </sheetData>
@@ -534,35 +564,35 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
+      <c r="A2" s="3"/>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>